<commit_message>
small commit towards Climbing Enhancing
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Pirates Game</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t xml:space="preserve">save point for leaving the game </t>
+  </si>
+  <si>
+    <t>Input fixing</t>
+  </si>
+  <si>
+    <t>Installing Net Code</t>
   </si>
 </sst>
 </file>
@@ -216,13 +222,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G18"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -537,7 +546,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
@@ -673,7 +682,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
@@ -684,7 +693,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
@@ -694,6 +703,159 @@
       <c r="D18" s="1" t="s">
         <v>45</v>
       </c>
+    </row>
+    <row r="26" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45342</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45343</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>3</v>
+      </c>
+      <c r="B28" s="3">
+        <v>45344</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3">
+        <v>45345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>5</v>
+      </c>
+      <c r="B30" s="3">
+        <v>45346</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>6</v>
+      </c>
+      <c r="B31" s="3">
+        <v>45347</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3">
+        <v>45348</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>8</v>
+      </c>
+      <c r="B33" s="3">
+        <v>45349</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>9</v>
+      </c>
+      <c r="B34" s="3">
+        <v>45350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>10</v>
+      </c>
+      <c r="B35" s="3">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>11</v>
+      </c>
+      <c r="B36" s="3">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3">
+        <v>45353</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>13</v>
+      </c>
+      <c r="B38" s="3">
+        <v>45354</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>14</v>
+      </c>
+      <c r="B39" s="3">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>15</v>
+      </c>
+      <c r="B40" s="3">
+        <v>45356</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>16</v>
+      </c>
+      <c r="B41" s="3">
+        <v>45357</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>17</v>
+      </c>
+      <c r="B42" s="3">
+        <v>45358</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>18</v>
+      </c>
+      <c r="B43" s="3">
+        <v>45359</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>